<commit_message>
added try/cach block to catch exceptions
</commit_message>
<xml_diff>
--- a/Documentation/Scrum/Sprint3Burndown.xlsx
+++ b/Documentation/Scrum/Sprint3Burndown.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Resume state</t>
+  </si>
+  <si>
+    <t>Rest API</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1128,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="4">
         <v>0</v>
@@ -1577,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H12" s="4">
         <v>0</v>
@@ -1626,7 +1629,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="4">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4">
@@ -1664,13 +1667,13 @@
         <v>34</v>
       </c>
       <c r="F14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4">
         <v>0</v>
       </c>
       <c r="H14" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I14" s="4">
         <v>1</v>
@@ -1716,13 +1719,13 @@
         <v>0</v>
       </c>
       <c r="H15" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J15" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="4">
         <v>0</v>
@@ -1749,19 +1752,23 @@
       <c r="A16" s="1"/>
       <c r="B16" s="7"/>
       <c r="C16" s="10"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="F16" s="4">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4">
         <v>1</v>
       </c>
-      <c r="G16" s="4">
-        <v>0</v>
-      </c>
       <c r="H16" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="4">
         <v>0</v>
@@ -1856,7 +1863,7 @@
       </c>
       <c r="G18" s="4">
         <f t="shared" ref="G18:P18" si="1">F18 - SUM(G4:G13)</f>
-        <v>14</v>
+        <v>13.5</v>
       </c>
       <c r="H18" s="4">
         <f t="shared" si="1"/>
@@ -2444,30 +2451,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>False</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <DocumentBusinessValueTaxHTField0 xmlns="http://schemas.microsoft.com/sharepoint/v3">
@@ -2518,6 +2501,30 @@
     </DocumentStatusTaxHTField0>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>False</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events"/>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2750,30 +2757,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D14C1044-F523-4937-BF47-727729F19EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B20B8EA-C8C4-49B1-8280-945BA6550F81}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90C1BE12-9AF4-4D82-8933-6D42A4A8E2C9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2786,6 +2769,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="30a82cfc-8d0b-455e-b705-4035c60ff9fd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D6E300D-687F-49DD-9C99-AC5EA1BE3BF7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B20B8EA-C8C4-49B1-8280-945BA6550F81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D14C1044-F523-4937-BF47-727729F19EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>